<commit_message>
OtoDom - Dodanie wyjątków związanych z obsługą pliku arkusza kalkulacyjnego. Dodanie kolumny z datą do arkusza.
</commit_message>
<xml_diff>
--- a/oto-dom.xlsx
+++ b/oto-dom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Udemy\Python\oto-dom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B0E202-1F9D-4635-A112-6EF601341AE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3B92A3-E2E1-48DF-9F0C-56A1F8AC7EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Nazwa</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>https://www.otodom.pl/pl/oferta/blisko-placu-narutowicza-ID4gMm5.html</t>
+  </si>
+  <si>
+    <t>Data</t>
   </si>
 </sst>
 </file>
@@ -417,21 +420,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="94.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -439,40 +441,51 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="e">
+      <c r="C2" s="2" t="e">
+        <f ca="1">INDIRECT("'"&amp;$A2&amp;"'!A2")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D2" t="e">
         <f ca="1">INDIRECT("'"&amp;$A2&amp;"'!C2")</f>
         <v>#REF!</v>
       </c>
-      <c r="D2" t="e">
+      <c r="E2" t="e">
         <f ca="1">INDIRECT("'"&amp;$A2&amp;"'!E2")</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="e">
+      <c r="C3" s="2" t="e">
+        <f ca="1">INDIRECT("'"&amp;$A3&amp;"'!A2")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D3" t="e">
         <f ca="1">INDIRECT("'"&amp;$A3&amp;"'!C2")</f>
         <v>#REF!</v>
       </c>
-      <c r="D3" t="e">
+      <c r="E3" t="e">
         <f ca="1">INDIRECT("'"&amp;$A3&amp;"'!E2")</f>
         <v>#REF!</v>
       </c>

</xml_diff>